<commit_message>
Feat: Implementar suporte completo para PT-BR nos templates e upload
- Atualizar arquivos modelo CSV e Excel com valores em português
- Implementar mapeamento português  inglês na validação
- Adicionar conversão automática de valores PT-BR para EN
- Melhorar tratamento pós-upload com validação e progresso
- Atualizar instruções de uso com exemplos em português
- Adicionar feedback detalhado de erros e sucessos
- Implementar barra de progresso durante importação em lote
</commit_message>
<xml_diff>
--- a/frontend/public/templates/prompts-template.xlsx
+++ b/frontend/public/templates/prompts-template.xlsx
@@ -403,10 +403,10 @@
   </sheetViews>
   <cols>
     <col min="1" max="1" width="25.83203125" customWidth="1"/>
-    <col min="2" max="2" width="15.83203125" customWidth="1"/>
-    <col min="3" max="3" width="15.83203125" customWidth="1"/>
+    <col min="2" max="2" width="20.83203125" customWidth="1"/>
+    <col min="3" max="3" width="20.83203125" customWidth="1"/>
     <col min="4" max="4" width="40.83203125" customWidth="1"/>
-    <col min="5" max="5" width="10.83203125" customWidth="1"/>
+    <col min="5" max="5" width="15.83203125" customWidth="1"/>
     <col min="6" max="6" width="15.83203125" customWidth="1"/>
     <col min="7" max="7" width="15.83203125" customWidth="1"/>
     <col min="8" max="8" width="30.83203125" customWidth="1"/>
@@ -471,22 +471,22 @@
         <v>Pergunta sobre experiência</v>
       </c>
       <c r="B2" t="str">
-        <v>INTERVIEW</v>
+        <v>Entrevista</v>
       </c>
       <c r="C2" t="str">
-        <v>FOLLOW_UP</v>
+        <v>Pergunta de Acompanhamento</v>
       </c>
       <c r="D2" t="str">
         <v>Conte-me sobre sua experiência anterior em atendimento ao cliente.</v>
       </c>
       <c r="E2" t="str">
-        <v>pt-BR</v>
+        <v>Português (Brasil)</v>
       </c>
       <c r="F2" t="str">
-        <v>PROFESSIONAL</v>
+        <v>Profissional</v>
       </c>
       <c r="G2" t="str">
-        <v>NEUTRAL</v>
+        <v>Neutro</v>
       </c>
       <c r="H2" t="str">
         <v>Usado na fase inicial da entrevista para avaliar experiência prévia</v>
@@ -498,13 +498,13 @@
         <v>Clareza na comunicação, exemplos específicos, relevância da experiência</v>
       </c>
       <c r="K2" t="str">
-        <v>MEDIUM</v>
+        <v>Médio</v>
       </c>
       <c r="L2">
         <v>120</v>
       </c>
       <c r="M2" t="str">
-        <v>experiência, atendimento, cliente, trabalho anterior</v>
+        <v>experiência, atendimento, cliente</v>
       </c>
       <c r="N2">
         <v>1</v>
@@ -518,22 +518,22 @@
         <v>Avaliação de soft skills</v>
       </c>
       <c r="B3" t="str">
-        <v>INTERVIEW</v>
+        <v>Entrevista</v>
       </c>
       <c r="C3" t="str">
-        <v>EVALUATION</v>
+        <v>Avaliação</v>
       </c>
       <c r="D3" t="str">
         <v>Avalie as habilidades de comunicação e resolução de problemas do candidato.</v>
       </c>
       <c r="E3" t="str">
-        <v>pt-BR</v>
+        <v>Português (Brasil)</v>
       </c>
       <c r="F3" t="str">
-        <v>PROFESSIONAL</v>
+        <v>Profissional</v>
       </c>
       <c r="G3" t="str">
-        <v>ENCOURAGING</v>
+        <v>Encorajador</v>
       </c>
       <c r="H3" t="str">
         <v>Aplicado durante a análise final do candidato</v>
@@ -545,7 +545,7 @@
         <v>Comunicação clara, pensamento crítico, criatividade, trabalho em equipe</v>
       </c>
       <c r="K3" t="str">
-        <v>HARD</v>
+        <v>Difícil</v>
       </c>
       <c r="L3">
         <v>180</v>
@@ -565,22 +565,22 @@
         <v>Atendimento reativo</v>
       </c>
       <c r="B4" t="str">
-        <v>CUSTOMER_SERVICE</v>
+        <v>Atendimento ao Cliente</v>
       </c>
       <c r="C4" t="str">
-        <v>INITIAL_MESSAGE</v>
+        <v>Mensagem Inicial</v>
       </c>
       <c r="D4" t="str">
         <v>Como você lidaria com um cliente insatisfeito com nosso produto?</v>
       </c>
       <c r="E4" t="str">
-        <v>pt-BR</v>
+        <v>Português (Brasil)</v>
       </c>
       <c r="F4" t="str">
-        <v>FRIENDLY</v>
+        <v>Amigável</v>
       </c>
       <c r="G4" t="str">
-        <v>POSITIVE</v>
+        <v>Positivo</v>
       </c>
       <c r="H4" t="str">
         <v>Cenário de simulação para testar habilidades de atendimento</v>
@@ -592,7 +592,7 @@
         <v>Empatia, proatividade, conhecimento do produto, técnicas de resolução</v>
       </c>
       <c r="K4" t="str">
-        <v>MEDIUM</v>
+        <v>Médio</v>
       </c>
       <c r="L4">
         <v>150</v>
@@ -612,22 +612,22 @@
         <v>Venda consultiva</v>
       </c>
       <c r="B5" t="str">
-        <v>SALES</v>
+        <v>Vendas</v>
       </c>
       <c r="C5" t="str">
-        <v>FOLLOW_UP</v>
+        <v>Pergunta de Acompanhamento</v>
       </c>
       <c r="D5" t="str">
         <v>Demonstre como você faria uma venda consultiva para um produto complexo.</v>
       </c>
       <c r="E5" t="str">
-        <v>pt-BR</v>
+        <v>Português (Brasil)</v>
       </c>
       <c r="F5" t="str">
-        <v>PROFESSIONAL</v>
+        <v>Profissional</v>
       </c>
       <c r="G5" t="str">
-        <v>CHALLENGING</v>
+        <v>Desafiador</v>
       </c>
       <c r="H5" t="str">
         <v>Teste prático de habilidades de vendas consultivas</v>
@@ -639,7 +639,7 @@
         <v>Estrutura do processo, perguntas qualificadoras, handling de objeções</v>
       </c>
       <c r="K5" t="str">
-        <v>EXPERT</v>
+        <v>Especialista</v>
       </c>
       <c r="L5">
         <v>300</v>

</xml_diff>